<commit_message>
Updating MTB_stats.xlsx with Revel and Ibis bike data
</commit_message>
<xml_diff>
--- a/Data/mtb_stats.xlsx
+++ b/Data/mtb_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtschulberg\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56E88CF-4F33-4F24-965F-2E0A4F6F7B9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EA8B0C-14B7-4FA1-B383-610470AAD606}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="180" windowWidth="29040" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="585" uniqueCount="189">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -697,9 +697,6 @@
     <t>Sheet2</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>price</t>
   </si>
   <si>
@@ -761,6 +758,45 @@
   </si>
   <si>
     <t>handlebar_width</t>
+  </si>
+  <si>
+    <t>XG1</t>
+  </si>
+  <si>
+    <t>https://www.transitionbikes.com/WebStoreImages/2020_AdminProductImage_Spur_XO1_BlackPowder.jpg</t>
+  </si>
+  <si>
+    <t>https://www.transitionbikes.com/WebStoreImages/2021_AdminProductImage_SentinelCarbon_XO1_LoamGold.jpg</t>
+  </si>
+  <si>
+    <t>XX1 AXS EAGLE KIT</t>
+  </si>
+  <si>
+    <t>https://www.revelbikes.com/wp-content/uploads/2020/06/Ranger-_Johnny_Green_Jeans_Complete_3-4_Drive_Side_WEB.jpg</t>
+  </si>
+  <si>
+    <t>build_type</t>
+  </si>
+  <si>
+    <t>https://www.revelbikes.com/wp-content/uploads/2020/10/Rascal-Frame-Cosmic-Purple-Profile-WEB.jpg</t>
+  </si>
+  <si>
+    <t>XX1 EAGLE AXS KIT</t>
+  </si>
+  <si>
+    <t>https://www.revelbikes.com/wp-content/uploads/2022/03/image001_Cropped_2-980x664.jpg.webp</t>
+  </si>
+  <si>
+    <t>XX1</t>
+  </si>
+  <si>
+    <t>https://assets-ibiscycles-com.s3.amazonaws.com/images/Bikes/Exie/Builder/exie-build-xx1-1200.png</t>
+  </si>
+  <si>
+    <t>https://assets-ibiscycles-com.s3.amazonaws.com/images/Bikes/Ripmo-2/Builder/ripmo2-buildKit-xx1-axs-blue-july20.png</t>
+  </si>
+  <si>
+    <t>https://assets-ibiscycles-com.s3.amazonaws.com/images/Bikes/Ripley-4/Builder/ripley4-buildKit-xx1AXS-MY21-black-120621.png</t>
   </si>
 </sst>
 </file>
@@ -1168,7 +1204,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1260,6 +1296,8 @@
     <xf numFmtId="49" fontId="10" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="44" fontId="6" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="10" fillId="8" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -2180,7 +2218,7 @@
     <tableColumn id="1" xr3:uid="{94CB6E26-43BC-46C8-8694-13FE5211D135}" name="url" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{C48E4292-8767-42F8-9490-9C7034A87C65}" name="model" dataDxfId="27"/>
     <tableColumn id="3" xr3:uid="{E14A9B0B-28E2-4628-BCEE-024217EFC7BB}" name="brand" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{30D423AE-F8E6-4CDD-9F2D-30D92E20E05F}" name="type" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{30D423AE-F8E6-4CDD-9F2D-30D92E20E05F}" name="build_type" dataDxfId="25"/>
     <tableColumn id="5" xr3:uid="{D90E0A31-E32A-4122-B6A9-3FE17F04E177}" name="price" dataDxfId="24" dataCellStyle="Currency"/>
     <tableColumn id="26" xr3:uid="{479F50D8-0823-4E9E-B40E-C6F03C8D88AC}" name="image" dataDxfId="0" dataCellStyle="Currency"/>
     <tableColumn id="6" xr3:uid="{226DB6B5-CA1A-4404-84C3-651C46E1CEA4}" name="setting" dataDxfId="23"/>
@@ -3359,8 +3397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3395,7 +3433,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>6</v>
@@ -3403,14 +3441,14 @@
       <c r="C1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="78" t="s">
+        <v>181</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>155</v>
       </c>
-      <c r="E1" s="7" t="s">
-        <v>156</v>
-      </c>
       <c r="F1" s="78" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>8</v>
@@ -3452,7 +3490,7 @@
         <v>20</v>
       </c>
       <c r="T1" s="80" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="U1" s="7" t="s">
         <v>22</v>
@@ -6260,7 +6298,7 @@
         <v>82</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E44" s="69">
         <v>9799</v>
@@ -6326,7 +6364,7 @@
         <v>90</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E45" s="69">
         <v>10229</v>
@@ -6392,13 +6430,13 @@
         <v>94</v>
       </c>
       <c r="D46" s="75" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E46" s="69">
         <v>9499</v>
       </c>
       <c r="F46" s="69" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G46" s="28"/>
       <c r="H46" s="73" t="s">
@@ -6460,13 +6498,13 @@
         <v>94</v>
       </c>
       <c r="D47" s="76" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E47" s="68">
         <v>7499</v>
       </c>
       <c r="F47" s="79" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G47" s="16"/>
       <c r="H47" s="77" t="s">
@@ -6528,13 +6566,13 @@
         <v>100</v>
       </c>
       <c r="D48" s="75" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E48" s="69">
         <v>3999</v>
       </c>
       <c r="F48" s="69" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G48" s="28"/>
       <c r="H48" s="73" t="s">
@@ -6587,7 +6625,7 @@
     </row>
     <row r="49" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="47" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B49" s="27" t="s">
         <v>102</v>
@@ -6596,13 +6634,13 @@
         <v>103</v>
       </c>
       <c r="D49" s="27" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E49" s="69">
         <v>10999</v>
       </c>
       <c r="F49" s="69" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G49" s="28"/>
       <c r="H49" s="73" t="s">
@@ -6668,13 +6706,13 @@
         <v>103</v>
       </c>
       <c r="D50" s="27" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E50" s="69">
         <v>10499</v>
       </c>
       <c r="F50" s="69" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G50" s="28"/>
       <c r="H50" s="73" t="s">
@@ -6744,13 +6782,13 @@
         <v>103</v>
       </c>
       <c r="D51" s="27" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E51" s="69">
         <v>9999</v>
       </c>
       <c r="F51" s="69" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G51" s="28"/>
       <c r="H51" s="73" t="s">
@@ -6820,13 +6858,13 @@
         <v>103</v>
       </c>
       <c r="D52" s="27" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E52" s="69">
         <v>9499</v>
       </c>
       <c r="F52" s="69" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G52" s="28"/>
       <c r="H52" s="73" t="s">
@@ -6891,9 +6929,15 @@
       <c r="C53" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="D53" s="27"/>
-      <c r="E53" s="69"/>
-      <c r="F53" s="69"/>
+      <c r="D53" s="75" t="s">
+        <v>176</v>
+      </c>
+      <c r="E53" s="69">
+        <v>6499</v>
+      </c>
+      <c r="F53" s="69" t="s">
+        <v>177</v>
+      </c>
       <c r="G53" s="28"/>
       <c r="H53" s="27" t="s">
         <v>45</v>
@@ -6964,8 +7008,12 @@
         <v>111</v>
       </c>
       <c r="D54" s="15"/>
-      <c r="E54" s="68"/>
-      <c r="F54" s="68"/>
+      <c r="E54" s="68">
+        <v>7199</v>
+      </c>
+      <c r="F54" s="68" t="s">
+        <v>178</v>
+      </c>
       <c r="G54" s="16"/>
       <c r="H54" s="15" t="s">
         <v>45</v>
@@ -7107,31 +7155,69 @@
       <c r="C57" s="47" t="s">
         <v>125</v>
       </c>
-      <c r="D57" s="47"/>
-      <c r="E57" s="72"/>
-      <c r="F57" s="72"/>
+      <c r="D57" s="47" t="s">
+        <v>179</v>
+      </c>
+      <c r="E57" s="72">
+        <v>12099</v>
+      </c>
+      <c r="F57" s="72" t="s">
+        <v>180</v>
+      </c>
       <c r="G57" s="56"/>
-      <c r="H57" s="56"/>
+      <c r="H57" s="81" t="s">
+        <v>30</v>
+      </c>
       <c r="I57" s="57" t="s">
         <v>112</v>
       </c>
-      <c r="J57" s="58"/>
-      <c r="K57" s="58"/>
+      <c r="J57" s="58">
+        <v>115</v>
+      </c>
+      <c r="K57" s="58">
+        <v>120</v>
+      </c>
       <c r="L57" s="59"/>
-      <c r="M57" s="59"/>
+      <c r="M57" s="59">
+        <v>180</v>
+      </c>
       <c r="N57" s="59"/>
-      <c r="O57" s="59"/>
-      <c r="P57" s="60"/>
-      <c r="Q57" s="60"/>
-      <c r="R57" s="61"/>
-      <c r="S57" s="61"/>
-      <c r="T57" s="61"/>
-      <c r="U57" s="62"/>
-      <c r="V57" s="56"/>
-      <c r="W57" s="56"/>
-      <c r="X57" s="56"/>
-      <c r="Y57" s="56"/>
-      <c r="Z57" s="56"/>
+      <c r="O57" s="59">
+        <v>160</v>
+      </c>
+      <c r="P57" s="60">
+        <v>67.5</v>
+      </c>
+      <c r="Q57" s="60">
+        <v>75.3</v>
+      </c>
+      <c r="R57" s="61">
+        <v>170</v>
+      </c>
+      <c r="S57" s="61">
+        <v>40</v>
+      </c>
+      <c r="T57" s="61">
+        <v>780</v>
+      </c>
+      <c r="U57" s="62">
+        <v>473</v>
+      </c>
+      <c r="V57" s="56">
+        <v>619</v>
+      </c>
+      <c r="W57" s="56">
+        <v>1194</v>
+      </c>
+      <c r="X57" s="56">
+        <v>436</v>
+      </c>
+      <c r="Y57" s="56">
+        <v>338</v>
+      </c>
+      <c r="Z57" s="56">
+        <v>699</v>
+      </c>
     </row>
     <row r="58" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="47" t="s">
@@ -7143,31 +7229,67 @@
       <c r="C58" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="D58" s="47"/>
-      <c r="E58" s="72"/>
-      <c r="F58" s="72"/>
+      <c r="D58" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="E58" s="72">
+        <v>10999</v>
+      </c>
+      <c r="F58" s="72" t="s">
+        <v>182</v>
+      </c>
       <c r="G58" s="56"/>
-      <c r="H58" s="56"/>
+      <c r="H58" s="81" t="s">
+        <v>30</v>
+      </c>
       <c r="I58" s="57" t="s">
         <v>115</v>
       </c>
-      <c r="J58" s="58"/>
-      <c r="K58" s="58"/>
+      <c r="J58" s="58">
+        <v>130</v>
+      </c>
+      <c r="K58" s="58">
+        <v>140</v>
+      </c>
       <c r="L58" s="59"/>
       <c r="M58" s="59"/>
       <c r="N58" s="59"/>
-      <c r="O58" s="59"/>
-      <c r="P58" s="60"/>
-      <c r="Q58" s="60"/>
-      <c r="R58" s="61"/>
-      <c r="S58" s="61"/>
-      <c r="T58" s="61"/>
-      <c r="U58" s="62"/>
-      <c r="V58" s="56"/>
-      <c r="W58" s="56"/>
-      <c r="X58" s="56"/>
-      <c r="Y58" s="56"/>
-      <c r="Z58" s="56"/>
+      <c r="O58" s="59">
+        <v>180</v>
+      </c>
+      <c r="P58" s="60">
+        <v>66</v>
+      </c>
+      <c r="Q58" s="60">
+        <v>75</v>
+      </c>
+      <c r="R58" s="61">
+        <v>170</v>
+      </c>
+      <c r="S58" s="61">
+        <v>40</v>
+      </c>
+      <c r="T58" s="61">
+        <v>780</v>
+      </c>
+      <c r="U58" s="62">
+        <v>464</v>
+      </c>
+      <c r="V58" s="56">
+        <v>618</v>
+      </c>
+      <c r="W58" s="56">
+        <v>1220</v>
+      </c>
+      <c r="X58" s="56">
+        <v>433</v>
+      </c>
+      <c r="Y58" s="56">
+        <v>335</v>
+      </c>
+      <c r="Z58" s="56">
+        <v>716</v>
+      </c>
     </row>
     <row r="59" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="47" t="s">
@@ -7179,11 +7301,19 @@
       <c r="C59" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="D59" s="47"/>
-      <c r="E59" s="72"/>
-      <c r="F59" s="72"/>
+      <c r="D59" s="47" t="s">
+        <v>183</v>
+      </c>
+      <c r="E59" s="72">
+        <v>10999</v>
+      </c>
+      <c r="F59" s="72" t="s">
+        <v>184</v>
+      </c>
       <c r="G59" s="56"/>
-      <c r="H59" s="56"/>
+      <c r="H59" s="81" t="s">
+        <v>30</v>
+      </c>
       <c r="I59" s="57" t="s">
         <v>119</v>
       </c>
@@ -7192,18 +7322,42 @@
       <c r="L59" s="59"/>
       <c r="M59" s="59"/>
       <c r="N59" s="59"/>
-      <c r="O59" s="59"/>
-      <c r="P59" s="60"/>
-      <c r="Q59" s="60"/>
-      <c r="R59" s="61"/>
-      <c r="S59" s="61"/>
-      <c r="T59" s="61"/>
-      <c r="U59" s="62"/>
-      <c r="V59" s="56"/>
-      <c r="W59" s="56"/>
-      <c r="X59" s="56"/>
-      <c r="Y59" s="56"/>
-      <c r="Z59" s="56"/>
+      <c r="O59" s="59">
+        <v>180</v>
+      </c>
+      <c r="P59" s="60">
+        <v>65</v>
+      </c>
+      <c r="Q59" s="60">
+        <v>76</v>
+      </c>
+      <c r="R59" s="61">
+        <v>270</v>
+      </c>
+      <c r="S59" s="61">
+        <v>40</v>
+      </c>
+      <c r="T59" s="61">
+        <v>800</v>
+      </c>
+      <c r="U59" s="62">
+        <v>469</v>
+      </c>
+      <c r="V59" s="56">
+        <v>637</v>
+      </c>
+      <c r="W59" s="56">
+        <v>1228</v>
+      </c>
+      <c r="X59" s="56">
+        <v>436</v>
+      </c>
+      <c r="Y59" s="56">
+        <v>348</v>
+      </c>
+      <c r="Z59" s="56">
+        <v>728</v>
+      </c>
     </row>
     <row r="60" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="47" t="s">
@@ -7215,11 +7369,19 @@
       <c r="C60" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="D60" s="47"/>
-      <c r="E60" s="72"/>
-      <c r="F60" s="72"/>
+      <c r="D60" s="82" t="s">
+        <v>185</v>
+      </c>
+      <c r="E60" s="72">
+        <v>12799</v>
+      </c>
+      <c r="F60" s="72" t="s">
+        <v>186</v>
+      </c>
       <c r="G60" s="56"/>
-      <c r="H60" s="56"/>
+      <c r="H60" s="81" t="s">
+        <v>30</v>
+      </c>
       <c r="I60" s="57" t="s">
         <v>84</v>
       </c>
@@ -7229,21 +7391,49 @@
       <c r="K60" s="63">
         <v>120</v>
       </c>
-      <c r="L60" s="59"/>
-      <c r="M60" s="59"/>
-      <c r="N60" s="59"/>
-      <c r="O60" s="59"/>
-      <c r="P60" s="60"/>
-      <c r="Q60" s="60"/>
-      <c r="R60" s="61"/>
-      <c r="S60" s="61"/>
-      <c r="T60" s="61"/>
-      <c r="U60" s="62"/>
-      <c r="V60" s="56"/>
-      <c r="W60" s="56"/>
-      <c r="X60" s="56"/>
+      <c r="L60" s="59">
+        <v>2</v>
+      </c>
+      <c r="M60" s="59">
+        <v>180</v>
+      </c>
+      <c r="N60" s="59">
+        <v>2</v>
+      </c>
+      <c r="O60" s="59">
+        <v>160</v>
+      </c>
+      <c r="P60" s="60">
+        <v>67.2</v>
+      </c>
+      <c r="Q60" s="60">
+        <v>74.8</v>
+      </c>
+      <c r="R60" s="61">
+        <v>175</v>
+      </c>
+      <c r="S60" s="61">
+        <v>50</v>
+      </c>
+      <c r="T60" s="61">
+        <v>780</v>
+      </c>
+      <c r="U60" s="62">
+        <v>478</v>
+      </c>
+      <c r="V60" s="56">
+        <v>606</v>
+      </c>
+      <c r="W60" s="56">
+        <v>1202</v>
+      </c>
+      <c r="X60" s="56">
+        <v>435</v>
+      </c>
       <c r="Y60" s="56"/>
-      <c r="Z60" s="56"/>
+      <c r="Z60" s="56">
+        <v>748</v>
+      </c>
     </row>
     <row r="61" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="47" t="s">
@@ -7255,11 +7445,19 @@
       <c r="C61" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="D61" s="47"/>
-      <c r="E61" s="72"/>
-      <c r="F61" s="72"/>
+      <c r="D61" s="82" t="s">
+        <v>185</v>
+      </c>
+      <c r="E61" s="72">
+        <v>11699</v>
+      </c>
+      <c r="F61" s="72" t="s">
+        <v>187</v>
+      </c>
       <c r="G61" s="56"/>
-      <c r="H61" s="56"/>
+      <c r="H61" s="81" t="s">
+        <v>30</v>
+      </c>
       <c r="I61" s="57" t="s">
         <v>87</v>
       </c>
@@ -7269,21 +7467,51 @@
       <c r="K61" s="63">
         <v>160</v>
       </c>
-      <c r="L61" s="59"/>
-      <c r="M61" s="59"/>
-      <c r="N61" s="59"/>
-      <c r="O61" s="59"/>
-      <c r="P61" s="60"/>
-      <c r="Q61" s="60"/>
-      <c r="R61" s="61"/>
-      <c r="S61" s="61"/>
-      <c r="T61" s="61"/>
-      <c r="U61" s="62"/>
-      <c r="V61" s="56"/>
-      <c r="W61" s="56"/>
-      <c r="X61" s="56"/>
-      <c r="Y61" s="56"/>
-      <c r="Z61" s="56"/>
+      <c r="L61" s="59">
+        <v>4</v>
+      </c>
+      <c r="M61" s="59">
+        <v>200</v>
+      </c>
+      <c r="N61" s="59">
+        <v>4</v>
+      </c>
+      <c r="O61" s="59">
+        <v>180</v>
+      </c>
+      <c r="P61" s="60">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="Q61" s="60">
+        <v>76</v>
+      </c>
+      <c r="R61" s="61">
+        <v>175</v>
+      </c>
+      <c r="S61" s="61">
+        <v>50</v>
+      </c>
+      <c r="T61" s="61">
+        <v>780</v>
+      </c>
+      <c r="U61" s="62">
+        <v>475</v>
+      </c>
+      <c r="V61" s="56">
+        <v>628</v>
+      </c>
+      <c r="W61" s="56">
+        <v>1238</v>
+      </c>
+      <c r="X61" s="56">
+        <v>435</v>
+      </c>
+      <c r="Y61" s="56">
+        <v>341</v>
+      </c>
+      <c r="Z61" s="56">
+        <v>740</v>
+      </c>
     </row>
     <row r="62" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="47" t="s">
@@ -7295,11 +7523,19 @@
       <c r="C62" s="47" t="s">
         <v>133</v>
       </c>
-      <c r="D62" s="47"/>
-      <c r="E62" s="72"/>
-      <c r="F62" s="72"/>
+      <c r="D62" s="82" t="s">
+        <v>185</v>
+      </c>
+      <c r="E62" s="72">
+        <v>11499</v>
+      </c>
+      <c r="F62" s="72" t="s">
+        <v>188</v>
+      </c>
       <c r="G62" s="56"/>
-      <c r="H62" s="56"/>
+      <c r="H62" s="81" t="s">
+        <v>30</v>
+      </c>
       <c r="I62" s="57" t="s">
         <v>87</v>
       </c>
@@ -7309,21 +7545,51 @@
       <c r="K62" s="63">
         <v>130</v>
       </c>
-      <c r="L62" s="59"/>
-      <c r="M62" s="59"/>
-      <c r="N62" s="59"/>
-      <c r="O62" s="59"/>
-      <c r="P62" s="60"/>
-      <c r="Q62" s="60"/>
-      <c r="R62" s="61"/>
-      <c r="S62" s="61"/>
-      <c r="T62" s="61"/>
-      <c r="U62" s="62"/>
-      <c r="V62" s="56"/>
-      <c r="W62" s="56"/>
-      <c r="X62" s="56"/>
-      <c r="Y62" s="56"/>
-      <c r="Z62" s="56"/>
+      <c r="L62" s="59">
+        <v>2</v>
+      </c>
+      <c r="M62" s="59">
+        <v>180</v>
+      </c>
+      <c r="N62" s="59">
+        <v>2</v>
+      </c>
+      <c r="O62" s="59">
+        <v>180</v>
+      </c>
+      <c r="P62" s="60">
+        <v>66.55</v>
+      </c>
+      <c r="Q62" s="60">
+        <v>76</v>
+      </c>
+      <c r="R62" s="61">
+        <v>175</v>
+      </c>
+      <c r="S62" s="61">
+        <v>50</v>
+      </c>
+      <c r="T62" s="61">
+        <v>780</v>
+      </c>
+      <c r="U62" s="62">
+        <v>475</v>
+      </c>
+      <c r="V62" s="56">
+        <v>622</v>
+      </c>
+      <c r="W62" s="56">
+        <v>1207</v>
+      </c>
+      <c r="X62" s="56">
+        <v>432</v>
+      </c>
+      <c r="Y62" s="56">
+        <v>335</v>
+      </c>
+      <c r="Z62" s="56">
+        <v>742</v>
+      </c>
     </row>
     <row r="63" spans="1:26" ht="15.4" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="47" t="s">

</xml_diff>